<commit_message>
added pandas HDF5 example
</commit_message>
<xml_diff>
--- a/src/16 Scientific Libraries/07 Spreadsheets/data/calendar.xlsx
+++ b/src/16 Scientific Libraries/07 Spreadsheets/data/calendar.xlsx
@@ -500,7 +500,7 @@
       <c r="D2" s="1" t="inlineStr"/>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>January</t>
+          <t>JANUARY</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr"/>
@@ -511,7 +511,7 @@
       <c r="L2" s="1" t="inlineStr"/>
       <c r="M2" s="2" t="inlineStr">
         <is>
-          <t>January</t>
+          <t>JANUARY</t>
         </is>
       </c>
       <c r="N2" s="1" t="inlineStr"/>
@@ -816,7 +816,7 @@
       <c r="D10" s="1" t="inlineStr"/>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>FEBRUARY</t>
         </is>
       </c>
       <c r="F10" s="1" t="inlineStr"/>
@@ -827,7 +827,7 @@
       <c r="L10" s="1" t="inlineStr"/>
       <c r="M10" s="2" t="inlineStr">
         <is>
-          <t>February</t>
+          <t>FEBRUARY</t>
         </is>
       </c>
       <c r="N10" s="1" t="inlineStr"/>
@@ -1124,7 +1124,7 @@
       <c r="D18" s="1" t="inlineStr"/>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>MARCH</t>
         </is>
       </c>
       <c r="F18" s="1" t="inlineStr"/>
@@ -1135,7 +1135,7 @@
       <c r="L18" s="1" t="inlineStr"/>
       <c r="M18" s="2" t="inlineStr">
         <is>
-          <t>March</t>
+          <t>MARCH</t>
         </is>
       </c>
       <c r="N18" s="1" t="inlineStr"/>
@@ -1440,7 +1440,7 @@
       <c r="D26" s="1" t="inlineStr"/>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>APRIL</t>
         </is>
       </c>
       <c r="F26" s="1" t="inlineStr"/>
@@ -1451,7 +1451,7 @@
       <c r="L26" s="1" t="inlineStr"/>
       <c r="M26" s="2" t="inlineStr">
         <is>
-          <t>April</t>
+          <t>APRIL</t>
         </is>
       </c>
       <c r="N26" s="1" t="inlineStr"/>
@@ -1752,7 +1752,7 @@
       <c r="D34" s="1" t="inlineStr"/>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>MAY</t>
         </is>
       </c>
       <c r="F34" s="1" t="inlineStr"/>
@@ -1763,7 +1763,7 @@
       <c r="L34" s="1" t="inlineStr"/>
       <c r="M34" s="2" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>MAY</t>
         </is>
       </c>
       <c r="N34" s="1" t="inlineStr"/>
@@ -2068,7 +2068,7 @@
       <c r="D42" s="1" t="inlineStr"/>
       <c r="E42" s="2" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>JUNE</t>
         </is>
       </c>
       <c r="F42" s="1" t="inlineStr"/>
@@ -2079,7 +2079,7 @@
       <c r="L42" s="1" t="inlineStr"/>
       <c r="M42" s="2" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>JUNE</t>
         </is>
       </c>
       <c r="N42" s="1" t="inlineStr"/>
@@ -2380,7 +2380,7 @@
       <c r="D50" s="1" t="inlineStr"/>
       <c r="E50" s="2" t="inlineStr">
         <is>
-          <t>July</t>
+          <t>JULY</t>
         </is>
       </c>
       <c r="F50" s="1" t="inlineStr"/>
@@ -2391,7 +2391,7 @@
       <c r="L50" s="1" t="inlineStr"/>
       <c r="M50" s="2" t="inlineStr">
         <is>
-          <t>July</t>
+          <t>JULY</t>
         </is>
       </c>
       <c r="N50" s="1" t="inlineStr"/>
@@ -2696,7 +2696,7 @@
       <c r="D58" s="1" t="inlineStr"/>
       <c r="E58" s="2" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>AUGUST</t>
         </is>
       </c>
       <c r="F58" s="1" t="inlineStr"/>
@@ -2707,7 +2707,7 @@
       <c r="L58" s="1" t="inlineStr"/>
       <c r="M58" s="2" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>AUGUST</t>
         </is>
       </c>
       <c r="N58" s="1" t="inlineStr"/>
@@ -3012,7 +3012,7 @@
       <c r="D66" s="1" t="inlineStr"/>
       <c r="E66" s="2" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>SEPTEMBER</t>
         </is>
       </c>
       <c r="F66" s="1" t="inlineStr"/>
@@ -3023,7 +3023,7 @@
       <c r="L66" s="1" t="inlineStr"/>
       <c r="M66" s="2" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>SEPTEMBER</t>
         </is>
       </c>
       <c r="N66" s="1" t="inlineStr"/>
@@ -3340,7 +3340,7 @@
       <c r="D75" s="1" t="inlineStr"/>
       <c r="E75" s="2" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>OCTOBER</t>
         </is>
       </c>
       <c r="F75" s="1" t="inlineStr"/>
@@ -3351,7 +3351,7 @@
       <c r="L75" s="1" t="inlineStr"/>
       <c r="M75" s="2" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>OCTOBER</t>
         </is>
       </c>
       <c r="N75" s="1" t="inlineStr"/>
@@ -3656,7 +3656,7 @@
       <c r="D83" s="1" t="inlineStr"/>
       <c r="E83" s="2" t="inlineStr">
         <is>
-          <t>November</t>
+          <t>NOVEMBER</t>
         </is>
       </c>
       <c r="F83" s="1" t="inlineStr"/>
@@ -3667,7 +3667,7 @@
       <c r="L83" s="1" t="inlineStr"/>
       <c r="M83" s="2" t="inlineStr">
         <is>
-          <t>November</t>
+          <t>NOVEMBER</t>
         </is>
       </c>
       <c r="N83" s="1" t="inlineStr"/>
@@ -3968,7 +3968,7 @@
       <c r="D91" s="1" t="inlineStr"/>
       <c r="E91" s="2" t="inlineStr">
         <is>
-          <t>December</t>
+          <t>DECEMBER</t>
         </is>
       </c>
       <c r="F91" s="1" t="inlineStr"/>
@@ -3979,7 +3979,7 @@
       <c r="L91" s="1" t="inlineStr"/>
       <c r="M91" s="2" t="inlineStr">
         <is>
-          <t>December</t>
+          <t>DECEMBER</t>
         </is>
       </c>
       <c r="N91" s="1" t="inlineStr"/>

</xml_diff>